<commit_message>
Sheet 3 Yerli Parçalar
Added new sheet for Özdisan components
</commit_message>
<xml_diff>
--- a/[05] PCB Design/ELE713-Hardware-List.xlsx
+++ b/[05] PCB Design/ELE713-Hardware-List.xlsx
@@ -1,18 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macit\Documents\GitHub\ELE713-SwitchedPowerSupplies\[05] PCB Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186B0827-E9E4-42A2-A3B9-24C9DAD698C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="251">
   <si>
     <t>Part Number</t>
   </si>
@@ -696,74 +706,152 @@
   </si>
   <si>
     <t>61.9kR 0603</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/mosfets/discrete-mosfets/CSD19534Q5A/594986</t>
+  </si>
+  <si>
+    <t>Özdisan Link veya TR</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/precision-power-and-shunt-resistors/SMK-R010-1-0/536411</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/integrated-circuits-ics/power-management-ics/linear-voltage-regulators/MC78M12CDTRKG/353490</t>
+  </si>
+  <si>
+    <t>MC78M12CDTRKG</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/optoelectronics/optocouplers-photocouplers-and-optics/optocoupler-logic-output/HCPL-M601-000E/709996</t>
+  </si>
+  <si>
+    <t>HCPL-M601-000E</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/precision-power-and-shunt-resistors/VMS-R047-1-0-U/536795</t>
+  </si>
+  <si>
+    <t>VMS-R047-1.0-U</t>
+  </si>
+  <si>
+    <t>SMK-R010-1.0</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/integrated-circuits-ics/power-management-ics/linear-voltage-regulators/MC7812CDTRKG/603063</t>
+  </si>
+  <si>
+    <t>MC7812CDTRKG</t>
+  </si>
+  <si>
+    <t>CSD18563Q5A</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/CSD18563Q5A?gad_source=1&amp;gclid=Cj0KCQiA1Km7BhC9ARIsAFZfEIvFuXxLwk3evw4lwW3L3bpncwkXR75VeoEu7y0iHbaem72N4-FDDb4aArFXEALw_wcB
+https://ozdisan.com/power-semiconductors/mosfets/discrete-mosfets/CSD18540Q5B/582556</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/p/854?ids=9693;354941,10311;413112,9976;368472&amp;groupids=9693,10311,9976&amp;propids=354941,413112,368472&amp;inStock=true&amp;sayfaAdedi=100</t>
+  </si>
+  <si>
+    <t>IXFY36N20X3</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/Product/Detail/38953/MBR0540T1G</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/transistors/discrete-transistors/BCX56-16115/344591</t>
+  </si>
+  <si>
+    <t>BCX56-16,115</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/diodes-diode-modules-and-rectifiers/general-purpose-diodes/BAS516115/529620</t>
+  </si>
+  <si>
+    <t>BAS516,115</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/power-semiconductors/diodes-diode-modules-and-rectifiers/schottky-diodes/SBA140CSR100001/574222</t>
+  </si>
+  <si>
+    <t>SBA140CS_R1_00001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Inherit"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -771,9 +859,33 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -787,8 +899,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -798,65 +912,76 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1046,29 +1171,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="33.13"/>
-    <col customWidth="1" min="3" max="3" width="23.0"/>
-    <col customWidth="1" min="4" max="4" width="19.88"/>
-    <col customWidth="1" min="5" max="5" width="12.25"/>
-    <col customWidth="1" min="6" max="6" width="16.38"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1102,13 +1231,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1122,13 +1251,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -1142,13 +1271,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="7">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1162,13 +1291,13 @@
         <v>9</v>
       </c>
       <c r="E5" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -1182,13 +1311,13 @@
         <v>9</v>
       </c>
       <c r="E6" s="7">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1202,13 +1331,13 @@
         <v>9</v>
       </c>
       <c r="E7" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -1222,13 +1351,13 @@
         <v>9</v>
       </c>
       <c r="E8" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
@@ -1242,13 +1371,13 @@
         <v>9</v>
       </c>
       <c r="E9" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -1262,13 +1391,13 @@
         <v>9</v>
       </c>
       <c r="E10" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -1282,13 +1411,13 @@
         <v>9</v>
       </c>
       <c r="E11" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
@@ -1302,13 +1431,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>51</v>
       </c>
@@ -1322,13 +1451,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>55</v>
       </c>
@@ -1342,13 +1471,13 @@
         <v>9</v>
       </c>
       <c r="E14" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>59</v>
       </c>
@@ -1362,13 +1491,13 @@
         <v>9</v>
       </c>
       <c r="E15" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>63</v>
       </c>
@@ -1382,13 +1511,13 @@
         <v>9</v>
       </c>
       <c r="E16" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>67</v>
       </c>
@@ -1402,13 +1531,13 @@
         <v>9</v>
       </c>
       <c r="E17" s="4">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>70</v>
       </c>
@@ -1422,13 +1551,13 @@
         <v>9</v>
       </c>
       <c r="E18" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1442,13 +1571,13 @@
         <v>9</v>
       </c>
       <c r="E19" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>78</v>
       </c>
@@ -1462,13 +1591,13 @@
         <v>9</v>
       </c>
       <c r="E20" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>82</v>
       </c>
@@ -1476,13 +1605,13 @@
         <v>83</v>
       </c>
       <c r="E21" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="10" t="s">
         <v>85</v>
       </c>
@@ -1493,13 +1622,13 @@
         <v>87</v>
       </c>
       <c r="E22" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>89</v>
       </c>
@@ -1510,13 +1639,13 @@
         <v>91</v>
       </c>
       <c r="E23" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>93</v>
       </c>
@@ -1524,13 +1653,13 @@
         <v>94</v>
       </c>
       <c r="E24" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>96</v>
       </c>
@@ -1544,13 +1673,13 @@
         <v>99</v>
       </c>
       <c r="E25" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>101</v>
       </c>
@@ -1561,13 +1690,13 @@
         <v>103</v>
       </c>
       <c r="E26" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="12" t="s">
         <v>105</v>
       </c>
@@ -1575,13 +1704,13 @@
         <v>106</v>
       </c>
       <c r="E27" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>108</v>
       </c>
@@ -1589,13 +1718,13 @@
         <v>109</v>
       </c>
       <c r="E28" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>111</v>
       </c>
@@ -1603,13 +1732,13 @@
         <v>112</v>
       </c>
       <c r="E29" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>114</v>
       </c>
@@ -1617,13 +1746,13 @@
         <v>115</v>
       </c>
       <c r="E30" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>117</v>
       </c>
@@ -1631,13 +1760,13 @@
         <v>118</v>
       </c>
       <c r="E31" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>120</v>
       </c>
@@ -1645,13 +1774,13 @@
         <v>121</v>
       </c>
       <c r="E32" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>123</v>
       </c>
@@ -1659,13 +1788,13 @@
         <v>124</v>
       </c>
       <c r="E33" s="4">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>126</v>
       </c>
@@ -1673,13 +1802,13 @@
         <v>127</v>
       </c>
       <c r="E34" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>129</v>
       </c>
@@ -1687,13 +1816,13 @@
         <v>130</v>
       </c>
       <c r="E35" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>132</v>
       </c>
@@ -1701,13 +1830,13 @@
         <v>133</v>
       </c>
       <c r="E36" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>135</v>
       </c>
@@ -1715,13 +1844,13 @@
         <v>136</v>
       </c>
       <c r="E37" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>138</v>
       </c>
@@ -1729,13 +1858,13 @@
         <v>139</v>
       </c>
       <c r="E38" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>141</v>
       </c>
@@ -1743,13 +1872,13 @@
         <v>142</v>
       </c>
       <c r="E39" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>144</v>
       </c>
@@ -1757,13 +1886,13 @@
         <v>145</v>
       </c>
       <c r="E40" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>147</v>
       </c>
@@ -1771,13 +1900,13 @@
         <v>148</v>
       </c>
       <c r="E41" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>150</v>
       </c>
@@ -1785,13 +1914,13 @@
         <v>151</v>
       </c>
       <c r="E42" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>152</v>
       </c>
@@ -1799,13 +1928,13 @@
         <v>153</v>
       </c>
       <c r="E43" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>155</v>
       </c>
@@ -1813,13 +1942,13 @@
         <v>156</v>
       </c>
       <c r="E44" s="4">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>158</v>
       </c>
@@ -1833,15 +1962,15 @@
         <v>159</v>
       </c>
       <c r="E45" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -2796,98 +2925,94 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="C3"/>
-    <hyperlink r:id="rId5" ref="B4"/>
-    <hyperlink r:id="rId6" ref="C4"/>
-    <hyperlink r:id="rId7" ref="B5"/>
-    <hyperlink r:id="rId8" ref="C5"/>
-    <hyperlink r:id="rId9" ref="B6"/>
-    <hyperlink r:id="rId10" ref="C6"/>
-    <hyperlink r:id="rId11" ref="B7"/>
-    <hyperlink r:id="rId12" ref="C7"/>
-    <hyperlink r:id="rId13" ref="B8"/>
-    <hyperlink r:id="rId14" ref="C8"/>
-    <hyperlink r:id="rId15" ref="B9"/>
-    <hyperlink r:id="rId16" ref="C9"/>
-    <hyperlink r:id="rId17" ref="B10"/>
-    <hyperlink r:id="rId18" ref="C10"/>
-    <hyperlink r:id="rId19" ref="B11"/>
-    <hyperlink r:id="rId20" ref="C11"/>
-    <hyperlink r:id="rId21" ref="B12"/>
-    <hyperlink r:id="rId22" ref="C12"/>
-    <hyperlink r:id="rId23" ref="B13"/>
-    <hyperlink r:id="rId24" ref="C13"/>
-    <hyperlink r:id="rId25" ref="B14"/>
-    <hyperlink r:id="rId26" ref="C14"/>
-    <hyperlink r:id="rId27" ref="B15"/>
-    <hyperlink r:id="rId28" ref="C15"/>
-    <hyperlink r:id="rId29" ref="B16"/>
-    <hyperlink r:id="rId30" ref="C16"/>
-    <hyperlink r:id="rId31" ref="B17"/>
-    <hyperlink r:id="rId32" ref="C17"/>
-    <hyperlink r:id="rId33" ref="B18"/>
-    <hyperlink r:id="rId34" ref="C18"/>
-    <hyperlink r:id="rId35" ref="B19"/>
-    <hyperlink r:id="rId36" ref="C19"/>
-    <hyperlink r:id="rId37" ref="B20"/>
-    <hyperlink r:id="rId38" ref="C20"/>
-    <hyperlink r:id="rId39" ref="C21"/>
-    <hyperlink r:id="rId40" ref="B22"/>
-    <hyperlink r:id="rId41" ref="C22"/>
-    <hyperlink r:id="rId42" ref="B23"/>
-    <hyperlink r:id="rId43" ref="C23"/>
-    <hyperlink r:id="rId44" ref="B24"/>
-    <hyperlink r:id="rId45" ref="B25"/>
-    <hyperlink r:id="rId46" ref="C25"/>
-    <hyperlink r:id="rId47" ref="D25"/>
-    <hyperlink r:id="rId48" ref="B26"/>
-    <hyperlink r:id="rId49" ref="D26"/>
-    <hyperlink r:id="rId50" ref="B27"/>
-    <hyperlink r:id="rId51" ref="B28"/>
-    <hyperlink r:id="rId52" ref="B29"/>
-    <hyperlink r:id="rId53" ref="B30"/>
-    <hyperlink r:id="rId54" ref="B31"/>
-    <hyperlink r:id="rId55" ref="B32"/>
-    <hyperlink r:id="rId56" ref="B33"/>
-    <hyperlink r:id="rId57" ref="B34"/>
-    <hyperlink r:id="rId58" ref="B35"/>
-    <hyperlink r:id="rId59" ref="B36"/>
-    <hyperlink r:id="rId60" ref="B37"/>
-    <hyperlink r:id="rId61" ref="B38"/>
-    <hyperlink r:id="rId62" ref="B39"/>
-    <hyperlink r:id="rId63" ref="B40"/>
-    <hyperlink r:id="rId64" ref="B41"/>
-    <hyperlink r:id="rId65" ref="B42"/>
-    <hyperlink r:id="rId66" ref="B43"/>
-    <hyperlink r:id="rId67" ref="B44"/>
-    <hyperlink r:id="rId68" ref="D45"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B22" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C22" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B23" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C23" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B24" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B25" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C25" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D25" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B26" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D26" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B27" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B28" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B29" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B30" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B31" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B32" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B33" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B34" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B35" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B36" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B37" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B38" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B39" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B40" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B41" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B42" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B43" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B44" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="D45" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId69"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="25.75"/>
-    <col customWidth="1" min="6" max="6" width="37.75"/>
-    <col customWidth="1" min="7" max="26" width="8.63"/>
+    <col min="1" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="7" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1">
+    <row r="1" spans="1:11" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2907,7 +3032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
+    <row r="2" spans="1:11" ht="12.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>161</v>
       </c>
@@ -2915,13 +3040,13 @@
         <v>162</v>
       </c>
       <c r="E2" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1">
+    <row r="3" spans="1:11" ht="12.75" customHeight="1">
       <c r="A3" s="13" t="s">
         <v>164</v>
       </c>
@@ -2929,13 +3054,13 @@
         <v>165</v>
       </c>
       <c r="E3" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>167</v>
       </c>
@@ -2943,13 +3068,13 @@
         <v>168</v>
       </c>
       <c r="E4" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" ht="12.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>170</v>
       </c>
@@ -2957,13 +3082,13 @@
         <v>171</v>
       </c>
       <c r="E5" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" ht="12.75" customHeight="1">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="13" t="s">
         <v>173</v>
       </c>
@@ -2971,13 +3096,13 @@
         <v>174</v>
       </c>
       <c r="E6" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
@@ -2985,13 +3110,13 @@
         <v>176</v>
       </c>
       <c r="E7" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="13" t="s">
         <v>43</v>
       </c>
@@ -2999,13 +3124,13 @@
         <v>44</v>
       </c>
       <c r="E8" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" ht="12.75" customHeight="1">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="13" t="s">
         <v>177</v>
       </c>
@@ -3013,13 +3138,13 @@
         <v>178</v>
       </c>
       <c r="E9" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" ht="12.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>51</v>
       </c>
@@ -3033,13 +3158,13 @@
         <v>9</v>
       </c>
       <c r="E10" s="4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" ht="12.75" customHeight="1">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -3053,13 +3178,13 @@
         <v>9</v>
       </c>
       <c r="E11" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="12" ht="12.75" customHeight="1">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -3073,13 +3198,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="13" ht="12.75" customHeight="1">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
@@ -3093,13 +3218,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" ht="12.75" customHeight="1">
+    <row r="14" spans="1:11" ht="12.75" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -3113,13 +3238,13 @@
         <v>9</v>
       </c>
       <c r="E14" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="15" ht="12.75" customHeight="1">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -3133,13 +3258,13 @@
         <v>9</v>
       </c>
       <c r="E15" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" ht="12.75" customHeight="1">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -3153,7 +3278,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>185</v>
@@ -3162,7 +3287,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" ht="12.75" customHeight="1">
+    <row r="17" spans="1:6" ht="12.75" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
@@ -3176,13 +3301,13 @@
         <v>9</v>
       </c>
       <c r="E17" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="18" ht="12.75" customHeight="1">
+    <row r="18" spans="1:6" ht="12.75" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -3196,13 +3321,13 @@
         <v>9</v>
       </c>
       <c r="E18" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="19" ht="12.75" customHeight="1">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
@@ -3216,13 +3341,13 @@
         <v>9</v>
       </c>
       <c r="E19" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
+    <row r="20" spans="1:6" ht="12.75" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>9</v>
       </c>
@@ -3236,13 +3361,13 @@
         <v>9</v>
       </c>
       <c r="E20" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" ht="12.75" customHeight="1">
+    <row r="21" spans="1:6" ht="12.75" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
@@ -3256,13 +3381,13 @@
         <v>9</v>
       </c>
       <c r="E21" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" ht="12.75" customHeight="1">
+    <row r="22" spans="1:6" ht="12.75" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
@@ -3276,13 +3401,13 @@
         <v>9</v>
       </c>
       <c r="E22" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" ht="12.75" customHeight="1">
+    <row r="23" spans="1:6" ht="12.75" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -3296,13 +3421,13 @@
         <v>9</v>
       </c>
       <c r="E23" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="24" ht="12.75" customHeight="1">
+    <row r="24" spans="1:6" ht="12.75" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>9</v>
       </c>
@@ -3316,13 +3441,13 @@
         <v>9</v>
       </c>
       <c r="E24" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="25" ht="12.75" customHeight="1">
+    <row r="25" spans="1:6" ht="12.75" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
@@ -3336,13 +3461,13 @@
         <v>9</v>
       </c>
       <c r="E25" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="26" ht="12.75" customHeight="1">
+    <row r="26" spans="1:6" ht="12.75" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>9</v>
       </c>
@@ -3356,13 +3481,13 @@
         <v>9</v>
       </c>
       <c r="E26" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="27" ht="12.75" customHeight="1">
+    <row r="27" spans="1:6" ht="12.75" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
@@ -3376,13 +3501,13 @@
         <v>9</v>
       </c>
       <c r="E27" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="28" ht="12.75" customHeight="1">
+    <row r="28" spans="1:6" ht="12.75" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>9</v>
       </c>
@@ -3396,13 +3521,13 @@
         <v>9</v>
       </c>
       <c r="E28" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="29" ht="12.75" customHeight="1">
+    <row r="29" spans="1:6" ht="12.75" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>9</v>
       </c>
@@ -3416,13 +3541,13 @@
         <v>9</v>
       </c>
       <c r="E29" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="30" ht="12.75" customHeight="1">
+    <row r="30" spans="1:6" ht="12.75" customHeight="1">
       <c r="A30" s="6" t="s">
         <v>9</v>
       </c>
@@ -3436,13 +3561,13 @@
         <v>9</v>
       </c>
       <c r="E30" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="31" ht="12.75" customHeight="1">
+    <row r="31" spans="1:6" ht="12.75" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>9</v>
       </c>
@@ -3456,13 +3581,13 @@
         <v>9</v>
       </c>
       <c r="E31" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="32" ht="12.75" customHeight="1">
+    <row r="32" spans="1:6" ht="12.75" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>9</v>
       </c>
@@ -3476,13 +3601,13 @@
         <v>9</v>
       </c>
       <c r="E32" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="33" ht="12.75" customHeight="1">
+    <row r="33" spans="1:6" ht="12.75" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>9</v>
       </c>
@@ -3496,13 +3621,13 @@
         <v>9</v>
       </c>
       <c r="E33" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="34" ht="12.75" customHeight="1">
+    <row r="34" spans="1:6" ht="12.75" customHeight="1">
       <c r="A34" s="6" t="s">
         <v>9</v>
       </c>
@@ -3516,13 +3641,13 @@
         <v>9</v>
       </c>
       <c r="E34" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="35" ht="12.75" customHeight="1">
+    <row r="35" spans="1:6" ht="12.75" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>9</v>
       </c>
@@ -3536,13 +3661,13 @@
         <v>9</v>
       </c>
       <c r="E35" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
+    <row r="36" spans="1:6" ht="12.75" customHeight="1">
       <c r="A36" s="6" t="s">
         <v>9</v>
       </c>
@@ -3556,13 +3681,13 @@
         <v>9</v>
       </c>
       <c r="E36" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="37" ht="12.75" customHeight="1">
+    <row r="37" spans="1:6" ht="12.75" customHeight="1">
       <c r="A37" s="6" t="s">
         <v>9</v>
       </c>
@@ -3576,13 +3701,13 @@
         <v>9</v>
       </c>
       <c r="E37" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="38" ht="12.75" customHeight="1">
+    <row r="38" spans="1:6" ht="12.75" customHeight="1">
       <c r="A38" s="6" t="s">
         <v>9</v>
       </c>
@@ -3596,13 +3721,13 @@
         <v>9</v>
       </c>
       <c r="E38" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
+    <row r="39" spans="1:6" ht="12.75" customHeight="1">
       <c r="A39" s="6" t="s">
         <v>9</v>
       </c>
@@ -3616,13 +3741,13 @@
         <v>9</v>
       </c>
       <c r="E39" s="13">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="40" ht="12.75" customHeight="1">
+    <row r="40" spans="1:6" ht="12.75" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>9</v>
       </c>
@@ -3636,13 +3761,13 @@
         <v>9</v>
       </c>
       <c r="E40" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="41" ht="12.75" customHeight="1">
+    <row r="41" spans="1:6" ht="12.75" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>9</v>
       </c>
@@ -3656,13 +3781,13 @@
         <v>9</v>
       </c>
       <c r="E41" s="13">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="42" ht="12.75" customHeight="1">
+    <row r="42" spans="1:6" ht="12.75" customHeight="1">
       <c r="A42" s="13" t="s">
         <v>212</v>
       </c>
@@ -3670,13 +3795,13 @@
         <v>213</v>
       </c>
       <c r="E42" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="43" ht="12.75" customHeight="1">
+    <row r="43" spans="1:6" ht="12.75" customHeight="1">
       <c r="A43" s="13" t="s">
         <v>215</v>
       </c>
@@ -3684,13 +3809,13 @@
         <v>216</v>
       </c>
       <c r="E43" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F43" s="13" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="44" ht="12.75" customHeight="1">
+    <row r="44" spans="1:6" ht="12.75" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>9</v>
       </c>
@@ -3704,13 +3829,13 @@
         <v>9</v>
       </c>
       <c r="E44" s="13">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="45" ht="12.75" customHeight="1">
+    <row r="45" spans="1:6" ht="12.75" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>9</v>
       </c>
@@ -3724,13 +3849,13 @@
         <v>9</v>
       </c>
       <c r="E45" s="13">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="46" ht="12.75" customHeight="1">
+    <row r="46" spans="1:6" ht="12.75" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>9</v>
       </c>
@@ -3744,13 +3869,13 @@
         <v>9</v>
       </c>
       <c r="E46" s="13">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="47" ht="12.75" customHeight="1">
+    <row r="47" spans="1:6" ht="12.75" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>9</v>
       </c>
@@ -3764,13 +3889,13 @@
         <v>9</v>
       </c>
       <c r="E47" s="13">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="48" ht="12.75" customHeight="1">
+    <row r="48" spans="1:6" ht="12.75" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>9</v>
       </c>
@@ -3784,13 +3909,13 @@
         <v>9</v>
       </c>
       <c r="E48" s="13">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="49" ht="12.75" customHeight="1">
+    <row r="49" spans="1:6" ht="12.75" customHeight="1">
       <c r="A49" s="6" t="s">
         <v>9</v>
       </c>
@@ -3804,13 +3929,13 @@
         <v>9</v>
       </c>
       <c r="E49" s="13">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="50" ht="12.75" customHeight="1">
+    <row r="50" spans="1:6" ht="12.75" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>9</v>
       </c>
@@ -3824,13 +3949,13 @@
         <v>9</v>
       </c>
       <c r="E50" s="13">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="51" ht="12.75" customHeight="1">
+    <row r="51" spans="1:6" ht="12.75" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>9</v>
       </c>
@@ -3844,13 +3969,13 @@
         <v>9</v>
       </c>
       <c r="E51" s="13">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="52" ht="12.75" customHeight="1">
+    <row r="52" spans="1:6" ht="12.75" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>9</v>
       </c>
@@ -3864,13 +3989,13 @@
         <v>9</v>
       </c>
       <c r="E52" s="13">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="53" ht="12.75" customHeight="1">
+    <row r="53" spans="1:6" ht="12.75" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>9</v>
       </c>
@@ -3884,23 +4009,23 @@
         <v>9</v>
       </c>
       <c r="E53" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="54" ht="12.75" customHeight="1"/>
-    <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
-    <row r="58" ht="12.75" customHeight="1"/>
-    <row r="59" ht="12.75" customHeight="1"/>
-    <row r="60" ht="12.75" customHeight="1"/>
-    <row r="61" ht="12.75" customHeight="1"/>
-    <row r="62" ht="12.75" customHeight="1"/>
-    <row r="63" ht="12.75" customHeight="1"/>
-    <row r="64" ht="12.75" customHeight="1"/>
+    <row r="54" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="55" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="56" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="57" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="58" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="59" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="60" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="61" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="62" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="63" spans="1:6" ht="12.75" customHeight="1"/>
+    <row r="64" spans="1:6" ht="12.75" customHeight="1"/>
     <row r="65" ht="12.75" customHeight="1"/>
     <row r="66" ht="12.75" customHeight="1"/>
     <row r="67" ht="12.75" customHeight="1"/>
@@ -4839,22 +4964,703 @@
     <row r="1000" ht="12.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B8"/>
-    <hyperlink r:id="rId8" ref="B9"/>
-    <hyperlink r:id="rId9" ref="B10"/>
-    <hyperlink r:id="rId10" ref="C10"/>
-    <hyperlink r:id="rId11" ref="B42"/>
-    <hyperlink r:id="rId12" ref="B43"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B42" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="B43" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F7823-E70A-4E8D-B451-269AE17FAEE0}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="112.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="25.5">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25.5">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="25.5">
+      <c r="A8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25.5">
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.25" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="24" customHeight="1">
+      <c r="A15" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="4">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C23" s="4">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" s="4">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="4">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="24">
+      <c r="A27" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="4">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="4">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="4">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C37" s="4">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="4">
+        <v>2</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="4">
+        <v>4</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="4">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="4">
+        <v>4</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="4">
+        <v>2</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{152426DA-9F74-43E9-947B-EFA9EB056D2A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{F1C1BA8F-86C7-4F7E-ADB1-E09D0D25B834}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{B8D02979-C66D-4683-BD07-D601098ED7BD}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{9BB2847F-B91F-434E-B41C-07F101D5E911}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{011A4BDC-61F4-4B12-8A17-8B350C3AD9D1}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{3FBCAF6A-4415-4932-9105-7F5ACCBE41CF}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{38A4ACFD-26C8-4BA6-9D06-BBE67C0E5B04}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{EE52DF50-58A2-44A1-883A-2BDA5CD829C9}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{3C534278-3DC1-4B4E-9C8F-0C81531F6965}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{51460921-DC25-4847-8156-E642C030198A}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{42F19579-0BF8-4789-87FB-6721AE04E0E6}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{7DEE917C-C313-49B5-8AC4-29B91451F8D8}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{A5844987-F2CF-4894-A060-C9ED22593609}"/>
+    <hyperlink ref="B20" r:id="rId14" xr:uid="{FD245165-E3D4-462E-9FF0-412151D15017}"/>
+    <hyperlink ref="B24" r:id="rId15" xr:uid="{84683C48-C7D4-4EFC-AEC3-26937F2789AF}"/>
+    <hyperlink ref="B26" r:id="rId16" xr:uid="{45A05607-FAC6-4CEC-A12B-4C4522E5ABB7}"/>
+    <hyperlink ref="B27" r:id="rId17" xr:uid="{A4F42924-BC1E-4E82-8F59-A4E934B24B4B}"/>
+    <hyperlink ref="B28" r:id="rId18" xr:uid="{AFB5E945-3B55-48A6-BBDD-270349B92961}"/>
+    <hyperlink ref="B29" r:id="rId19" xr:uid="{B185F261-77CE-4B1F-944C-9DCDF09A1091}"/>
+    <hyperlink ref="B31" r:id="rId20" xr:uid="{441E8BE5-660B-4E2B-9D78-854EEE3784A9}"/>
+    <hyperlink ref="B33" r:id="rId21" xr:uid="{9CB97B99-4257-4A22-B629-C77458AF611A}"/>
+    <hyperlink ref="B34" r:id="rId22" xr:uid="{6AB29380-0F1B-4A89-800F-7FF7F2F26298}"/>
+    <hyperlink ref="B35" r:id="rId23" xr:uid="{1EA98E9E-BCA2-4AD9-B805-F8459E1EBA63}"/>
+    <hyperlink ref="B38" r:id="rId24" xr:uid="{82C0C2E3-F2D3-4E96-81E0-D601C0E63C7D}"/>
+    <hyperlink ref="B39" r:id="rId25" xr:uid="{CAF97BBF-CC3A-491A-AAD1-AA3EFF191AC5}"/>
+    <hyperlink ref="B40" r:id="rId26" xr:uid="{57A1FCB2-5E02-4785-8F8B-63E663161E11}"/>
+    <hyperlink ref="B41" r:id="rId27" xr:uid="{22738326-F526-483F-BDBE-A2363F723952}"/>
+    <hyperlink ref="B42" r:id="rId28" xr:uid="{008B61AD-6980-48F3-8D90-4D5DB576BB56}"/>
+    <hyperlink ref="B43" r:id="rId29" xr:uid="{FDD3C3E1-1CF8-4736-A919-22D451948076}"/>
+    <hyperlink ref="B44" r:id="rId30" xr:uid="{7CDE5F05-8E5C-4783-B623-BB1874D6BC09}"/>
+    <hyperlink ref="B30" r:id="rId31" xr:uid="{C63FB96D-EF10-4F9E-A9D6-07B8FC26BF91}"/>
+    <hyperlink ref="B36" r:id="rId32" xr:uid="{0D3CE2FB-C5AD-4E2A-8AE9-F33E9F123BC7}"/>
+    <hyperlink ref="B37" r:id="rId33" xr:uid="{C02E04D0-D0C1-4521-9E27-682ADD3A2139}"/>
+    <hyperlink ref="B15" r:id="rId34" display="https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/CSD18563Q5A?gad_source=1&amp;gclid=Cj0KCQiA1Km7BhC9ARIsAFZfEIvFuXxLwk3evw4lwW3L3bpncwkXR75VeoEu7y0iHbaem72N4-FDDb4aArFXEALw_wcB" xr:uid="{5C2B6CA4-7979-4E7E-A3F9-9DD11E125E0D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[05] Bom update from local sellers
</commit_message>
<xml_diff>
--- a/[05] PCB Design/ELE713-Hardware-List.xlsx
+++ b/[05] PCB Design/ELE713-Hardware-List.xlsx
@@ -1,28 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macit\Documents\GitHub\ELE713-SwitchedPowerSupplies\[05] PCB Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\metup\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4B1406-5FC7-4685-8F80-24EC9D80D614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C534938-DA1A-4C52-BB93-E44507CF5710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4236" yWindow="5652" windowWidth="17280" windowHeight="9960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="296">
   <si>
     <t>Part Number</t>
   </si>
@@ -721,12 +732,6 @@
   </si>
   <si>
     <t>MC78M12CDTRKG</t>
-  </si>
-  <si>
-    <t>https://ozdisan.com/optoelectronics/optocouplers-photocouplers-and-optics/optocoupler-logic-output/HCPL-M601-000E/709996</t>
-  </si>
-  <si>
-    <t>HCPL-M601-000E</t>
   </si>
   <si>
     <t>https://ozdisan.com/passive-components/resistors/precision-power-and-shunt-resistors/VMS-R047-1-0-U/536795</t>
@@ -797,15 +802,134 @@
     <t>GRM32ER61A107ME20L-</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/kemet/A768MS107M1HLAE024/12704540
-https://ozdisan.com/p/1214?ids=12870;906806&amp;groupids=12870&amp;propids=906806&amp;inStock=true&amp;sayfaAdedi=20</t>
+    <t xml:space="preserve"> DO NOT NEED</t>
+  </si>
+  <si>
+    <t>SALVAGE</t>
+  </si>
+  <si>
+    <t>SPARE / SALVAGE</t>
+  </si>
+  <si>
+    <t>https://www.ozdisan.com/optoelektronikler/optoelektronikler/transistor-ve-fotovoltaik-cikisli-optokuplorler/TCMT1106?srsltid=AfmBOooG_F5UGTPgMpcxH79DTjRTOyaivfQtirWmV3_66KGTzc-CD7oA</t>
+  </si>
+  <si>
+    <t>TCMT1106</t>
+  </si>
+  <si>
+    <t>OPTOISOLATOR 3.75KV TRANS 4-SOP</t>
+  </si>
+  <si>
+    <t>ÖZDİSAN</t>
+  </si>
+  <si>
+    <t>MOSFET DIS.100V 50A N-CH VSONP-8</t>
+  </si>
+  <si>
+    <t>BOUGHT</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/circuit-protections/fuse-components/fuses/SET1500/473352</t>
+  </si>
+  <si>
+    <t>SET1500</t>
+  </si>
+  <si>
+    <t>FUSE SMD 5A 250V 6125 TIME-LAG</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/circuit-protections/fuse-components/fuses/0154005-DR/669001</t>
+  </si>
+  <si>
+    <t>0154005.DR</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/circuit-protections/fuse-components/fuses/0154010-DR/612871</t>
+  </si>
+  <si>
+    <t>0154010.DR</t>
+  </si>
+  <si>
+    <t>FUSE BOARD MOUNT 10A 125VDC 2-SMD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/circuit-protections/fuse-components/fuses/SFE1800/994485</t>
+  </si>
+  <si>
+    <t>SFE1800</t>
+  </si>
+  <si>
+    <t>FUSE SMD 8A 125V 2SMD FAST ACTING</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/resistors/precision-power-and-shunt-resistors/CMS-R020-1-0/582282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS-R020-1.0 </t>
+  </si>
+  <si>
+    <t>RES.SHUNT (6432) 2512 20m Ohms 1% 2.5W AUTO SMT</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/aluminum-capacitors/VR-035V181MG126-TR/585021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VR-035V181MG126-T/R </t>
+  </si>
+  <si>
+    <t>CAP.EL.180uF 35V 10x12.6 MM 105C 2000H SMD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/aluminum-capacitors/VR-080V470MG126-TR/956356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VR-080V470MG126-T/R </t>
+  </si>
+  <si>
+    <t>CAP.EL.47uF 80V 10x12.60 105C 2000Hrs SMD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/inductors/fixed-inductors/SRI1209-100M/530619</t>
+  </si>
+  <si>
+    <t>INDUCTOR POWER 10UH 12X12MM SMD</t>
+  </si>
+  <si>
+    <t>SRI1209-100M</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/inductors/fixed-inductors/IHLP5050FDER100M01/589695</t>
+  </si>
+  <si>
+    <t>IHLP5050FDER100M01</t>
+  </si>
+  <si>
+    <t>INDUCTOR FIXED 10uH 20% SMD</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/MC20KTB251225/1201518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC20KTB251225 </t>
+  </si>
+  <si>
+    <t>MLCC (5750) 2220 2.2uF 250VDC ±10% X7R</t>
+  </si>
+  <si>
+    <t>https://ozdisan.com/passive-components/capacitors/smt-smd-and-mlcc-capacitors/CL31C221JIHNNNE/523539</t>
+  </si>
+  <si>
+    <t>CL31C221JIHNNNE</t>
+  </si>
+  <si>
+    <t>MLCC (3216) 1206 220pF 1000VDC ±5% C0G (NP0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -868,8 +992,32 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -884,24 +1032,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -944,12 +1122,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -961,10 +1191,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -977,23 +1203,75 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1210,23 +1488,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1246,187 +1524,196 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="21">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="21">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="21">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="21">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="21">
         <v>2</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="18">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="18">
         <v>2</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="18">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="18">
         <v>1</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -1446,7 +1733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
@@ -1466,7 +1753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>51</v>
       </c>
@@ -1486,7 +1773,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>55</v>
       </c>
@@ -1502,11 +1789,11 @@
       <c r="E14" s="4">
         <v>2</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>59</v>
       </c>
@@ -1526,7 +1813,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>63</v>
       </c>
@@ -1627,7 +1914,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1636,12 +1923,12 @@
       <c r="E21" s="4">
         <v>1</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1653,7 +1940,7 @@
       <c r="E22" s="4">
         <v>5</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1670,7 +1957,7 @@
       <c r="E23" s="4">
         <v>4</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1689,7 +1976,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1709,7 +1996,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
         <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1726,7 +2013,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1809,7 +2096,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1">
+    <row r="33" spans="1:9" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>123</v>
       </c>
@@ -1823,7 +2110,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>126</v>
       </c>
@@ -1837,7 +2124,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>129</v>
       </c>
@@ -1851,7 +2138,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1">
+    <row r="36" spans="1:9" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>132</v>
       </c>
@@ -1865,7 +2152,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1">
+    <row r="37" spans="1:9" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>135</v>
       </c>
@@ -1879,7 +2166,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+    <row r="38" spans="1:9" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>138</v>
       </c>
@@ -1893,7 +2180,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+    <row r="39" spans="1:9" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>141</v>
       </c>
@@ -1907,7 +2194,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1">
+    <row r="40" spans="1:9" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>144</v>
       </c>
@@ -1921,7 +2208,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1">
+    <row r="41" spans="1:9" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>147</v>
       </c>
@@ -1935,7 +2222,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1">
+    <row r="42" spans="1:9" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>150</v>
       </c>
@@ -1949,7 +2236,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1">
+    <row r="43" spans="1:9" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>152</v>
       </c>
@@ -1963,7 +2250,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1">
+    <row r="44" spans="1:9" ht="15.75" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>155</v>
       </c>
@@ -1977,29 +2264,32 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A45" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="5" t="s">
+      <c r="B45" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="15">
         <v>2</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="15" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:9" ht="15.75" customHeight="1"/>
+    <row r="48" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -3032,13 +3322,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" customWidth="1"/>
-    <col min="7" max="26" width="8.5703125" customWidth="1"/>
+    <col min="1" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
+    <col min="7" max="26" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1">
@@ -3062,114 +3354,114 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="11">
         <v>1</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>1</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <v>2</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <v>1</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <v>1</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="11">
         <v>2</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3206,10 +3498,10 @@
       <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="11">
         <v>2</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="13" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3226,10 +3518,10 @@
       <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="11">
         <v>2</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="13" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3246,7 +3538,7 @@
       <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <v>3</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -3266,7 +3558,7 @@
       <c r="D14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="11">
         <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -3286,7 +3578,7 @@
       <c r="D15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>3</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -3306,13 +3598,13 @@
       <c r="D16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <v>3</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="K16" s="16" t="s">
+      <c r="K16" s="14" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3329,7 +3621,7 @@
       <c r="D17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>1</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -3349,7 +3641,7 @@
       <c r="D18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -3369,7 +3661,7 @@
       <c r="D19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <v>1</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -3389,7 +3681,7 @@
       <c r="D20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="11">
         <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
@@ -3409,7 +3701,7 @@
       <c r="D21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <v>2</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -3429,7 +3721,7 @@
       <c r="D22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="11">
         <v>3</v>
       </c>
       <c r="F22" s="6" t="s">
@@ -3449,7 +3741,7 @@
       <c r="D23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="11">
         <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
@@ -3469,7 +3761,7 @@
       <c r="D24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="11">
         <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
@@ -3489,7 +3781,7 @@
       <c r="D25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="11">
         <v>2</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -3509,7 +3801,7 @@
       <c r="D26" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="11">
         <v>2</v>
       </c>
       <c r="F26" s="6" t="s">
@@ -3529,7 +3821,7 @@
       <c r="D27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="11">
         <v>1</v>
       </c>
       <c r="F27" s="6" t="s">
@@ -3549,7 +3841,7 @@
       <c r="D28" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="11">
         <v>1</v>
       </c>
       <c r="F28" s="6" t="s">
@@ -3569,7 +3861,7 @@
       <c r="D29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="11">
         <v>2</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -3589,7 +3881,7 @@
       <c r="D30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="11">
         <v>1</v>
       </c>
       <c r="F30" s="6" t="s">
@@ -3609,7 +3901,7 @@
       <c r="D31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="11">
         <v>1</v>
       </c>
       <c r="F31" s="6" t="s">
@@ -3629,7 +3921,7 @@
       <c r="D32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="11">
         <v>2</v>
       </c>
       <c r="F32" s="6" t="s">
@@ -3649,7 +3941,7 @@
       <c r="D33" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="11">
         <v>2</v>
       </c>
       <c r="F33" s="6" t="s">
@@ -3669,7 +3961,7 @@
       <c r="D34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="11">
         <v>1</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -3689,7 +3981,7 @@
       <c r="D35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="11">
         <v>1</v>
       </c>
       <c r="F35" s="6" t="s">
@@ -3709,7 +4001,7 @@
       <c r="D36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="11">
         <v>1</v>
       </c>
       <c r="F36" s="6" t="s">
@@ -3729,7 +4021,7 @@
       <c r="D37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="11">
         <v>1</v>
       </c>
       <c r="F37" s="6" t="s">
@@ -3749,7 +4041,7 @@
       <c r="D38" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="11">
         <v>3</v>
       </c>
       <c r="F38" s="6" t="s">
@@ -3769,7 +4061,7 @@
       <c r="D39" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="11">
         <v>6</v>
       </c>
       <c r="F39" s="6" t="s">
@@ -3789,7 +4081,7 @@
       <c r="D40" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="11">
         <v>2</v>
       </c>
       <c r="F40" s="6" t="s">
@@ -3809,7 +4101,7 @@
       <c r="D41" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="11">
         <v>6</v>
       </c>
       <c r="F41" s="6" t="s">
@@ -3817,30 +4109,30 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="11">
         <v>3</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="11" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="11">
         <v>3</v>
       </c>
-      <c r="F43" s="13" t="s">
+      <c r="F43" s="11" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3857,7 +4149,7 @@
       <c r="D44" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="11">
         <v>15</v>
       </c>
       <c r="F44" s="6" t="s">
@@ -3877,7 +4169,7 @@
       <c r="D45" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="11">
         <v>50</v>
       </c>
       <c r="F45" s="6" t="s">
@@ -3897,7 +4189,7 @@
       <c r="D46" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="11">
         <v>5</v>
       </c>
       <c r="F46" s="6" t="s">
@@ -3917,7 +4209,7 @@
       <c r="D47" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47" s="11">
         <v>20</v>
       </c>
       <c r="F47" s="6" t="s">
@@ -3937,10 +4229,10 @@
       <c r="D48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48" s="11">
         <v>5</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="13" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3957,7 +4249,7 @@
       <c r="D49" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="11">
         <v>5</v>
       </c>
       <c r="F49" s="6" t="s">
@@ -3977,7 +4269,7 @@
       <c r="D50" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E50" s="11">
         <v>5</v>
       </c>
       <c r="F50" s="6" t="s">
@@ -3997,7 +4289,7 @@
       <c r="D51" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="11">
         <v>5</v>
       </c>
       <c r="F51" s="6" t="s">
@@ -4017,7 +4309,7 @@
       <c r="D52" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="13">
+      <c r="E52" s="11">
         <v>10</v>
       </c>
       <c r="F52" s="6" t="s">
@@ -4037,7 +4329,7 @@
       <c r="D53" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E53" s="11">
         <v>3</v>
       </c>
       <c r="F53" s="6" t="s">
@@ -5013,644 +5305,809 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17F7823-E70A-4E8D-B451-269AE17FAEE0}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="112.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="2" max="2" width="112.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="34" customFormat="1">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+    </row>
+    <row r="2" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="28">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="28">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.5">
-      <c r="A4" s="4" t="s">
+      <c r="F3" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="28">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="25.5">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="28">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4" t="s">
+      <c r="F5" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="28">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
+      <c r="F6" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="26">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="25.5">
-      <c r="A8" s="4" t="s">
+      <c r="F7" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A8" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="26">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5">
-      <c r="A9" s="4" t="s">
+      <c r="F8" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="26">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="25.5">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="26">
         <v>1</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="29" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.25" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="F10" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="15">
         <v>3</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="15">
         <v>3</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
+      <c r="F12" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="15">
         <v>2</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="18" t="s">
+      <c r="F13" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="43" customFormat="1">
+      <c r="A14" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="41">
+        <v>4</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="43" customFormat="1">
+      <c r="A15" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" s="41">
+        <v>4</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="43" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" s="41">
+        <v>6</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="30" customFormat="1">
+      <c r="A17" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="26">
+        <v>4</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="55" customFormat="1" ht="26.4">
+      <c r="A18" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>252</v>
+      </c>
+      <c r="C18" s="50">
+        <v>6</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="43" customFormat="1">
+      <c r="A19" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" s="41">
+        <v>5</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="43" customFormat="1">
+      <c r="A20" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" s="41">
+        <v>2</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="43" customFormat="1">
+      <c r="A21" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21" s="41">
+        <v>4</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="30" customFormat="1">
+      <c r="A22" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="26">
+        <v>1</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="43" customFormat="1">
+      <c r="A23" s="52" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="C23" s="41">
+        <v>5</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="43" customFormat="1">
+      <c r="A24" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" s="41">
+        <v>4</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="17" customFormat="1">
+      <c r="A25" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="43" customFormat="1">
+      <c r="A26" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="C26" s="41">
+        <v>4</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="43" customFormat="1">
+      <c r="A27" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27" s="41">
+        <v>3</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="43" customFormat="1">
+      <c r="A28" s="41" t="s">
+        <v>250</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>251</v>
+      </c>
+      <c r="C28" s="41">
+        <v>3</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="30" customFormat="1">
+      <c r="A29" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="26">
+        <v>2</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="43" customFormat="1">
+      <c r="A30" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="41">
+        <v>2</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="43" customFormat="1">
+      <c r="A31" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B31" s="51" t="s">
         <v>233</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C31" s="41">
         <v>2</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="24" customHeight="1">
-      <c r="A15" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="D31" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="43" customFormat="1">
+      <c r="A32" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="C32" s="41">
         <v>4</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="D32" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="43" customFormat="1">
+      <c r="A33" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="C33" s="41">
         <v>4</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5">
-      <c r="A17" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="D33" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="55" customFormat="1">
+      <c r="A34" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="50">
+        <v>1</v>
+      </c>
+      <c r="D34" s="50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="43" customFormat="1">
+      <c r="A35" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="C35" s="41">
+        <v>2</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="43" customFormat="1">
+      <c r="A36" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="C36" s="41">
+        <v>2</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="43" customFormat="1">
+      <c r="A37" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" s="41">
+        <v>2</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="F37" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="43" customFormat="1">
+      <c r="A38" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="C38" s="41">
+        <v>2</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="F38" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="30" customFormat="1">
+      <c r="A39" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="26">
+        <v>2</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="17" customFormat="1">
+      <c r="A40" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="15">
+        <v>1</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="43" customFormat="1">
+      <c r="A41" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="B41" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="C41" s="41">
         <v>6</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C18" s="4">
-        <v>5</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="D41" s="39" t="s">
+        <v>292</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="43" customFormat="1">
+      <c r="A42" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B42" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="C42" s="41">
+        <v>10</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="F42" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="43" customFormat="1">
+      <c r="A43" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="C43" s="41">
+        <v>1</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F43" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="43" customFormat="1">
+      <c r="A44" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44" s="41">
+        <v>1</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="F44" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="43" customFormat="1">
+      <c r="A45" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="B45" s="51" t="s">
+        <v>264</v>
+      </c>
+      <c r="C45" s="41">
+        <v>6</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="F45" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="43" customFormat="1">
+      <c r="A46" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="C46" s="41">
+        <v>12</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="F46" s="44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="49" customFormat="1">
+      <c r="A47" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="48">
         <v>2</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C20" s="4">
-        <v>4</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C22" s="4">
-        <v>5</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C23" s="4">
-        <v>4</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C25" s="4">
-        <v>4</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C27" s="4">
-        <v>3</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="C28" s="4">
-        <v>3</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="4">
-        <v>2</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C31" s="4">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C32" s="4">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="25.5">
-      <c r="A33" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="C33" s="4">
-        <v>3</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C34" s="4">
-        <v>2</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C35" s="4">
-        <v>1</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="C36" s="4">
-        <v>2</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="C37" s="4">
-        <v>2</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C38" s="4">
-        <v>2</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="4">
-        <v>2</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C41" s="4">
-        <v>4</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="4">
-        <v>1</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C43" s="4">
-        <v>4</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C44" s="4">
-        <v>4</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="4">
-        <v>2</v>
-      </c>
-      <c r="D45" s="4" t="s">
+      <c r="D47" s="48" t="s">
         <v>160</v>
+      </c>
+      <c r="F47" s="49" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -5667,27 +6124,27 @@
     <hyperlink ref="B11" r:id="rId10" xr:uid="{51460921-DC25-4847-8156-E642C030198A}"/>
     <hyperlink ref="B12" r:id="rId11" xr:uid="{42F19579-0BF8-4789-87FB-6721AE04E0E6}"/>
     <hyperlink ref="B13" r:id="rId12" xr:uid="{7DEE917C-C313-49B5-8AC4-29B91451F8D8}"/>
-    <hyperlink ref="B16" r:id="rId13" xr:uid="{A5844987-F2CF-4894-A060-C9ED22593609}"/>
-    <hyperlink ref="B24" r:id="rId14" xr:uid="{84683C48-C7D4-4EFC-AEC3-26937F2789AF}"/>
-    <hyperlink ref="B26" r:id="rId15" xr:uid="{45A05607-FAC6-4CEC-A12B-4C4522E5ABB7}"/>
-    <hyperlink ref="B29" r:id="rId16" xr:uid="{B185F261-77CE-4B1F-944C-9DCDF09A1091}"/>
-    <hyperlink ref="B31" r:id="rId17" xr:uid="{441E8BE5-660B-4E2B-9D78-854EEE3784A9}"/>
-    <hyperlink ref="B33" r:id="rId18" display="https://www.digikey.com/en/products/detail/kemet/A768MS107M1HLAE024/12704540" xr:uid="{9CB97B99-4257-4A22-B629-C77458AF611A}"/>
-    <hyperlink ref="B34" r:id="rId19" xr:uid="{6AB29380-0F1B-4A89-800F-7FF7F2F26298}"/>
-    <hyperlink ref="B35" r:id="rId20" xr:uid="{1EA98E9E-BCA2-4AD9-B805-F8459E1EBA63}"/>
-    <hyperlink ref="B38" r:id="rId21" xr:uid="{82C0C2E3-F2D3-4E96-81E0-D601C0E63C7D}"/>
-    <hyperlink ref="B39" r:id="rId22" xr:uid="{CAF97BBF-CC3A-491A-AAD1-AA3EFF191AC5}"/>
-    <hyperlink ref="B40" r:id="rId23" xr:uid="{57A1FCB2-5E02-4785-8F8B-63E663161E11}"/>
-    <hyperlink ref="B41" r:id="rId24" xr:uid="{22738326-F526-483F-BDBE-A2363F723952}"/>
-    <hyperlink ref="B42" r:id="rId25" xr:uid="{008B61AD-6980-48F3-8D90-4D5DB576BB56}"/>
-    <hyperlink ref="B43" r:id="rId26" xr:uid="{FDD3C3E1-1CF8-4736-A919-22D451948076}"/>
-    <hyperlink ref="B44" r:id="rId27" xr:uid="{7CDE5F05-8E5C-4783-B623-BB1874D6BC09}"/>
-    <hyperlink ref="B30" r:id="rId28" xr:uid="{C63FB96D-EF10-4F9E-A9D6-07B8FC26BF91}"/>
-    <hyperlink ref="B36" r:id="rId29" xr:uid="{0D3CE2FB-C5AD-4E2A-8AE9-F33E9F123BC7}"/>
-    <hyperlink ref="B37" r:id="rId30" xr:uid="{C02E04D0-D0C1-4521-9E27-682ADD3A2139}"/>
-    <hyperlink ref="B15" r:id="rId31" display="https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/CSD18563Q5A?gad_source=1&amp;gclid=Cj0KCQiA1Km7BhC9ARIsAFZfEIvFuXxLwk3evw4lwW3L3bpncwkXR75VeoEu7y0iHbaem72N4-FDDb4aArFXEALw_wcB" xr:uid="{5C2B6CA4-7979-4E7E-A3F9-9DD11E125E0D}"/>
-    <hyperlink ref="B17" r:id="rId32" display="https://ozdisan.com/power-semiconductors/mosfets/discrete-mosfets/IRFH5020TRPBF/519539" xr:uid="{4F72EEBF-5BF2-4D18-87E7-CFB8321B5342}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{A5844987-F2CF-4894-A060-C9ED22593609}"/>
+    <hyperlink ref="B25" r:id="rId14" xr:uid="{84683C48-C7D4-4EFC-AEC3-26937F2789AF}"/>
+    <hyperlink ref="B29" r:id="rId15" xr:uid="{B185F261-77CE-4B1F-944C-9DCDF09A1091}"/>
+    <hyperlink ref="B32" r:id="rId16" xr:uid="{9CB97B99-4257-4A22-B629-C77458AF611A}"/>
+    <hyperlink ref="B33" r:id="rId17" xr:uid="{6AB29380-0F1B-4A89-800F-7FF7F2F26298}"/>
+    <hyperlink ref="B34" r:id="rId18" xr:uid="{1EA98E9E-BCA2-4AD9-B805-F8459E1EBA63}"/>
+    <hyperlink ref="B39" r:id="rId19" xr:uid="{82C0C2E3-F2D3-4E96-81E0-D601C0E63C7D}"/>
+    <hyperlink ref="B40" r:id="rId20" xr:uid="{CAF97BBF-CC3A-491A-AAD1-AA3EFF191AC5}"/>
+    <hyperlink ref="B46" r:id="rId21" xr:uid="{FDD3C3E1-1CF8-4736-A919-22D451948076}"/>
+    <hyperlink ref="B30" r:id="rId22" xr:uid="{C63FB96D-EF10-4F9E-A9D6-07B8FC26BF91}"/>
+    <hyperlink ref="B35" r:id="rId23" xr:uid="{0D3CE2FB-C5AD-4E2A-8AE9-F33E9F123BC7}"/>
+    <hyperlink ref="B36" r:id="rId24" xr:uid="{C02E04D0-D0C1-4521-9E27-682ADD3A2139}"/>
+    <hyperlink ref="B16" r:id="rId25" display="https://ozdisan.com/guc-yari-iletkenleri/mosfetler/discrete-mosfetler/CSD18563Q5A?gad_source=1&amp;gclid=Cj0KCQiA1Km7BhC9ARIsAFZfEIvFuXxLwk3evw4lwW3L3bpncwkXR75VeoEu7y0iHbaem72N4-FDDb4aArFXEALw_wcB" xr:uid="{5C2B6CA4-7979-4E7E-A3F9-9DD11E125E0D}"/>
+    <hyperlink ref="B18" r:id="rId26" display="https://ozdisan.com/power-semiconductors/mosfets/discrete-mosfets/IRFH5020TRPBF/519539" xr:uid="{4F72EEBF-5BF2-4D18-87E7-CFB8321B5342}"/>
+    <hyperlink ref="B14" r:id="rId27" xr:uid="{8E20029B-E5C9-4A2F-B988-C4E6A3372E30}"/>
+    <hyperlink ref="B19" r:id="rId28" xr:uid="{1E5A8FCD-B756-449F-9542-A7DEF40BE222}"/>
+    <hyperlink ref="B21" r:id="rId29" xr:uid="{0C762DC3-269E-487C-B528-AEC859B5440B}"/>
+    <hyperlink ref="B20" r:id="rId30" xr:uid="{70562509-B5F4-4E31-AF4A-D81DC91FE9E4}"/>
+    <hyperlink ref="B43" r:id="rId31" xr:uid="{DB56C10B-2DEB-44B9-9A49-96832335A822}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>